<commit_message>
Changed file name and tried to display file.
</commit_message>
<xml_diff>
--- a/log_return.xlsx
+++ b/log_return.xlsx
@@ -512,7 +512,7 @@
         <v>0.00197108636341305</v>
       </c>
       <c r="D2" t="n">
-        <v>0.005254808727120871</v>
+        <v>0.005254824124932698</v>
       </c>
       <c r="E2" t="n">
         <v>0.01099480698051476</v>
@@ -550,7 +550,7 @@
         <v>0.01053977158753255</v>
       </c>
       <c r="D3" t="n">
-        <v>0.006758873492502773</v>
+        <v>0.006758889186647915</v>
       </c>
       <c r="E3" t="n">
         <v>0.004001271931348707</v>
@@ -626,7 +626,7 @@
         <v>0.01628199256703529</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02118292198362704</v>
+        <v>0.02118292165369563</v>
       </c>
       <c r="E5" t="n">
         <v>0.01450940810650679</v>
@@ -647,7 +647,7 @@
         <v>0.01677203006030942</v>
       </c>
       <c r="K5" t="n">
-        <v>0.03309746818482923</v>
+        <v>0.03309747016943895</v>
       </c>
       <c r="L5" t="n">
         <v>0.0343919514067877</v>
@@ -664,7 +664,7 @@
         <v>0.01000461020909869</v>
       </c>
       <c r="D6" t="n">
-        <v>0.009871603575487808</v>
+        <v>0.009871587778178608</v>
       </c>
       <c r="E6" t="n">
         <v>0.002508284200458843</v>
@@ -685,7 +685,7 @@
         <v>0.006881145895357607</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0001939044985007811</v>
+        <v>0.0001939044986965865</v>
       </c>
       <c r="L6" t="n">
         <v>0.007153032313127058</v>
@@ -702,19 +702,19 @@
         <v>0.02463562436285614</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01675415705023492</v>
+        <v>0.01675414052703364</v>
       </c>
       <c r="E7" t="n">
         <v>0.01003637370952996</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0186160330757359</v>
+        <v>0.01861603451639441</v>
       </c>
       <c r="G7" t="n">
         <v>0.01452745796210854</v>
       </c>
       <c r="H7" t="n">
-        <v>0.02159692872328666</v>
+        <v>0.02159692791260594</v>
       </c>
       <c r="I7" t="n">
         <v>0.02826940837329224</v>
@@ -723,7 +723,7 @@
         <v>0.03104783837562176</v>
       </c>
       <c r="K7" t="n">
-        <v>0.05077827949745548</v>
+        <v>0.05077827838538069</v>
       </c>
       <c r="L7" t="n">
         <v>0.03873307565744376</v>
@@ -740,19 +740,19 @@
         <v>0.01917546020735375</v>
       </c>
       <c r="D8" t="n">
-        <v>0.006917768673602063</v>
+        <v>0.006917768788591217</v>
       </c>
       <c r="E8" t="n">
         <v>0.01259212969131535</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01075234708051136</v>
+        <v>0.01075234709635373</v>
       </c>
       <c r="G8" t="n">
         <v>0.009067379914640957</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0149090789166255</v>
+        <v>0.0149090786400349</v>
       </c>
       <c r="I8" t="n">
         <v>0.02797031776501228</v>
@@ -761,7 +761,7 @@
         <v>0.01064936249132288</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0108680238349796</v>
+        <v>0.01086802161761603</v>
       </c>
       <c r="L8" t="n">
         <v>0.003455306189097905</v>

</xml_diff>